<commit_message>
updated code for micro restriction
</commit_message>
<xml_diff>
--- a/edi_matlab_micro/dinamicadados.xlsx
+++ b/edi_matlab_micro/dinamicadados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuodr\Documents\programaceira\decolagem2022\edi_matlab_micro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8C425D-E7AE-47CD-A9F0-5A2D719FD85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C718E02-555D-4ED3-BC76-E48692DA2A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle" sheetId="1" r:id="rId1"/>
@@ -856,7 +856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="179">
   <si>
     <t>Variável</t>
   </si>
@@ -1363,6 +1363,36 @@
   </si>
   <si>
     <t>CLmax</t>
+  </si>
+  <si>
+    <t>x_tdp</t>
+  </si>
+  <si>
+    <t>x_tdn</t>
+  </si>
+  <si>
+    <t>distância do CG até o TDP (m, positivo)</t>
+  </si>
+  <si>
+    <t>distância do CG até o TDN (m, positivo)</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>Coeficiente de atrito da pista (adimensional)</t>
+  </si>
+  <si>
+    <t>Sd</t>
+  </si>
+  <si>
+    <t>Distância da pista (m)</t>
+  </si>
+  <si>
+    <t>z_mesa</t>
+  </si>
+  <si>
+    <t>Altura da mesa (m)</t>
   </si>
 </sst>
 </file>
@@ -1749,7 +1779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1922,6 +1952,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4765,8 +4804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4835,7 +4874,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="42">
-        <v>5.0199999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>11</v>
@@ -4881,10 +4920,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780516B4-2B26-4515-B1EB-EE0E9A20E5B7}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" activeCellId="2" sqref="B14 C15 D16"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5007,13 +5046,16 @@
         <v>33</v>
       </c>
       <c r="B9" s="59">
-        <v>-6.1499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="42" t="s">
         <v>35</v>
+      </c>
+      <c r="H9">
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -5035,7 +5077,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="42">
-        <v>0.25</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>39</v>
@@ -5138,6 +5180,61 @@
       </c>
       <c r="H16" s="42" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="66">
+        <v>3.32E-2</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="66">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="66">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" s="66">
+        <v>4.2</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5149,13 +5246,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7FD063-05B3-470D-AA7D-6BE4832597D6}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5242,7 +5340,7 @@
         <v>65</v>
       </c>
       <c r="H3" s="42">
-        <v>5100</v>
+        <v>9500</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
@@ -5276,7 +5374,7 @@
         <v>67</v>
       </c>
       <c r="H4" s="42">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" s="39"/>
       <c r="J4" s="39"/>
@@ -5403,7 +5501,7 @@
       <c r="A9" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="50">
+      <c r="B9" s="67">
         <v>0.29852699999999999</v>
       </c>
       <c r="C9" s="41" t="s">
@@ -5424,7 +5522,7 @@
       <c r="A10" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="68">
         <v>4.4114000000000004</v>
       </c>
       <c r="C10" s="39"/>
@@ -5501,7 +5599,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="46">
-        <v>0.25000953674316401</v>
+        <v>0.25</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -5976,8 +6074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DD314E-C382-46AC-806D-7E5988604C2A}">
   <dimension ref="A1:AD297"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6010,14 +6108,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="11"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -8926,8 +9024,9 @@
       <c r="A38" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="16">
-        <v>0</v>
+      <c r="B38" s="51">
+        <f>Y38</f>
+        <v>5.1100000000000003</v>
       </c>
       <c r="C38" s="54">
         <v>0</v>
@@ -9889,12 +9988,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010026F0D136D79F25469E9BD90619CDB412" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4a869207c6945743f5de18208a2cfcba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f9188d7-3b18-4187-a3cb-7b6899b4ef8f" xmlns:ns3="85078965-a7f2-4dbb-adf6-2b7faeeb76ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89813893f4c0c91941f9d9d5434200cd" ns2:_="" ns3:_="">
     <xsd:import namespace="4f9188d7-3b18-4187-a3cb-7b6899b4ef8f"/>
@@ -10117,7 +10210,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -10126,16 +10219,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D6E2B2-1F78-45C8-93F5-31B8FF78EAA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51AA6EA-A3F6-4587-80EF-6E5C51392FC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10154,10 +10244,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BAFCAE4-A011-4769-B47E-67DBBC3AE6CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D6E2B2-1F78-45C8-93F5-31B8FF78EAA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated micro drag data
</commit_message>
<xml_diff>
--- a/edi_matlab_micro/dinamicadados.xlsx
+++ b/edi_matlab_micro/dinamicadados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuodr\Documents\programaceira\decolagem2022\edi_matlab_micro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A25356-0C65-4755-A0CA-29E7BCFDEF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768B3000-A6DC-48B2-A8BA-A27958F7B77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,9 @@
     <sheet name="Controle" sheetId="1" r:id="rId1"/>
     <sheet name="Geral" sheetId="2" r:id="rId2"/>
     <sheet name="Superficies" sheetId="3" r:id="rId3"/>
-    <sheet name="Derivadas" sheetId="4" r:id="rId4"/>
-    <sheet name="Tracao" sheetId="5" r:id="rId5"/>
+    <sheet name="Arrastos" sheetId="6" r:id="rId4"/>
+    <sheet name="Derivadas" sheetId="4" r:id="rId5"/>
+    <sheet name="Tracao" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -324,157 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{9819BBBE-F5AF-4CA9-9DA0-13777667E689}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Luis Nicolas Kuodrek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coeficiente 'a' da curva de CD
-CD = a * alfa^2 + b * alfa + c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{1B3CBC6C-2C04-494F-B251-75C69AE477ED}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Luis Nicolas Kuodrek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coeficiente 'a' da curva de CD
-CD = a * alfa^2 + b * alfa + c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{269DA53C-F470-417E-B0EF-2503E1F958B1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Luis Nicolas Kuodrek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coeficiente 'b' da curva de CD
-CD = a * alfa^2 + b * alfa + c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{D4B86BE1-7234-4F39-9832-47C8C84B268C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Luis Nicolas Kuodrek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coeficiente 'b' da curva de CD
-CD = a * alfa^2 + b * alfa + c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{8294ED0E-89E5-4529-970A-1F5F299B1119}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Luis Nicolas Kuodrek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coeficiente 'c' da curva de CD
-CD = a * alfa^2 + b * alfa + c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{C042C049-C320-42AE-BB3C-4C62907EA759}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Luis Nicolas Kuodrek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coeficiente 'c' da curva de CD
-CD = a * alfa^2 + b * alfa + c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{F1062C2B-27A4-4B26-B6C3-0419C30640F0}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{F1062C2B-27A4-4B26-B6C3-0419C30640F0}">
       <text>
         <r>
           <rPr>
@@ -503,6 +354,366 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Luis Nicolas Kuodrek</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{61E2625E-00C2-49B0-BA8B-854D18916575}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'a' da curva de CD parasita da asa
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{5BC2C86A-3F8E-4362-8C70-DA75AD43C7A0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'a' da curva de CD parasita do EH
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{D655BCD0-69F7-4B48-9936-011E7C32154D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'a' da curva de CD parasita da EV
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{432A3AC3-BF52-41E3-84E8-3277B18DEB91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'a' da curva de CD parasita da fuselagem
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{8675C8E6-C84B-4481-A93D-7AFAF140B0DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'b' da curva de CD parasita da asa
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{B938AF42-9D12-432A-AED6-D268430EAD7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'b' da curva de CD parasita do EH
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{6C0A2B50-5671-4A54-8321-130D84CA49E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'b' da curva de CD parasita do EV
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{46F07873-2885-4455-8033-F957E9FF4DC9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'b' da curva de CD parasita da fuselagem
+CDp = a * V + b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{16FE8F45-BD19-407C-B32F-6D1FDD317B4C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'a' da curva de CD
+CD = a * alfa^2 + b * alfa + c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{3DD2A200-42AD-44B5-89E4-DBD463CDE331}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'a' da curva de CD
+CD = a * alfa^2 + b * alfa + c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{CD980BB5-3923-46BD-AB7D-86AB92AC4AA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'b' da curva de CD
+CD = a * alfa^2 + b * alfa + c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{E05EE86D-0A5F-44CC-881E-37E25914444A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'b' da curva de CD
+CD = a * alfa^2 + b * alfa + c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{CEBBCA2A-A186-4B2D-B349-08D9C15D95D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'c' da curva de CD
+CD = a * alfa^2 + b * alfa + c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D5CBFCBD-5542-4AA0-A332-56D9B2DFF3DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Luis Nicolas Kuodrek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coeficiente 'c' da curva de CD
+CD = a * alfa^2 + b * alfa + c</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Lucas Crestani</author>
@@ -856,7 +1067,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="202">
   <si>
     <t>Variável</t>
   </si>
@@ -1095,24 +1306,6 @@
     <t>epsilon0</t>
   </si>
   <si>
-    <t>CDw_c1</t>
-  </si>
-  <si>
-    <t>CDh_c1</t>
-  </si>
-  <si>
-    <t>CDw_c2</t>
-  </si>
-  <si>
-    <t>CDh_c2</t>
-  </si>
-  <si>
-    <t>CDw_c3</t>
-  </si>
-  <si>
-    <t>CDh_c3</t>
-  </si>
-  <si>
     <t>xac</t>
   </si>
   <si>
@@ -1393,20 +1586,106 @@
   </si>
   <si>
     <t>z_inicial</t>
+  </si>
+  <si>
+    <t>Arrasto parasita - Asa</t>
+  </si>
+  <si>
+    <t>Arrasto parasita - EH</t>
+  </si>
+  <si>
+    <t>Arrasto parasita - EV</t>
+  </si>
+  <si>
+    <t>Arrasto parasita - Fuselagem</t>
+  </si>
+  <si>
+    <t>CDpw</t>
+  </si>
+  <si>
+    <t>CDph</t>
+  </si>
+  <si>
+    <t>CDpv</t>
+  </si>
+  <si>
+    <t>CDpf</t>
+  </si>
+  <si>
+    <t>CDpw_c1</t>
+  </si>
+  <si>
+    <t>CDph_c1</t>
+  </si>
+  <si>
+    <t>CDpv_c1</t>
+  </si>
+  <si>
+    <t>CDpt_c1</t>
+  </si>
+  <si>
+    <t>CDpw_c2</t>
+  </si>
+  <si>
+    <t>CDph_c2</t>
+  </si>
+  <si>
+    <t>CDpv_c2</t>
+  </si>
+  <si>
+    <t>CDpt_c2</t>
+  </si>
+  <si>
+    <t>Arrasto induzido - Asa</t>
+  </si>
+  <si>
+    <t>Arrasto induzido - EH</t>
+  </si>
+  <si>
+    <t>O arrasto da fuselagem tá muito grande. Verificar com aerodinâmica</t>
+  </si>
+  <si>
+    <t>CDiw_c1</t>
+  </si>
+  <si>
+    <t>CDih_c1</t>
+  </si>
+  <si>
+    <t>Os arrastos estão ponderados?</t>
+  </si>
+  <si>
+    <t>CDiw_c2</t>
+  </si>
+  <si>
+    <t>CDih_c2</t>
+  </si>
+  <si>
+    <t>CDiw_c3</t>
+  </si>
+  <si>
+    <t>CDih_c3</t>
+  </si>
+  <si>
+    <t>Alfa</t>
+  </si>
+  <si>
+    <t>CDw</t>
+  </si>
+  <si>
+    <t>CDh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1468,6 +1747,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1566,18 +1865,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1745,17 +2044,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="2" tint="-0.499984740745262"/>
       </left>
@@ -1775,11 +2063,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1896,19 +2223,10 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1923,7 +2241,7 @@
     <xf numFmtId="11" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1938,29 +2256,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="8" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="8" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2849,6 +3201,806 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arrastos!$N$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arrastos!$M$9:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arrastos!$N$9:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.6010910259559698E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2187473473968699E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0919240514946401E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2692049611380298E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6097589464372206E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8618752210485005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0365637454707798E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.101569555026123</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.112560467436968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99C6-4C06-8182-D2A66D761BBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="597273216"/>
+        <c:axId val="597273872"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="597273216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="597273872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="597273872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="597273216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arrastos!$Q$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.6592300962379703E-4"/>
+                  <c:y val="-0.39736913094196558"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arrastos!$P$9:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arrastos!$Q$9:$Q$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.2986457399112525E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9829656566044261E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0882939599435668E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2876983381822764E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5369892387654705E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6442681458535092E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8313311342148428E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5418721241993274E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5397317936440814E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F5C9-48E7-BA3F-982597B9D610}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="596865896"/>
+        <c:axId val="596864256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="596865896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596864256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="596864256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596865896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2890,6 +4042,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3961,6 +5193,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4039,6 +6303,83 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C983E53-A3E6-F18A-465B-03267A855468}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127254</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD934DE8-5939-76F6-0073-3AF607642CEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4840,7 +7181,7 @@
       <c r="A3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="53">
+      <c r="B3" s="50">
         <v>9.75</v>
       </c>
       <c r="C3" s="42" t="s">
@@ -4874,7 +7215,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="42">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>11</v>
@@ -4923,7 +7264,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4956,7 +7297,7 @@
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -4972,10 +7313,10 @@
       <c r="C3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="46">
         <v>1000</v>
       </c>
-      <c r="J3" s="48">
+      <c r="J3" s="47">
         <f t="shared" ref="J3" si="0">1.255*(1-(0.0065*I3/288.15))^(9.8061/(0.0065*287.05307))</f>
         <v>1.1131837599499996</v>
       </c>
@@ -5028,10 +7369,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="56">
         <v>0</v>
       </c>
       <c r="C8" s="42" t="s">
@@ -5042,10 +7383,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="56">
         <v>0</v>
       </c>
       <c r="C9" s="42" t="s">
@@ -5059,10 +7400,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="59">
+      <c r="B10" s="56">
         <v>0</v>
       </c>
       <c r="C10" s="42" t="s">
@@ -5073,7 +7414,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="56" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="42">
@@ -5087,7 +7428,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="56" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="42">
@@ -5101,10 +7442,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="62">
+      <c r="B13" s="57">
         <v>0</v>
       </c>
       <c r="C13" s="42" t="s">
@@ -5115,10 +7456,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="64">
+      <c r="B14" s="59">
         <f>928028.676*0.000001</f>
         <v>0.92802867599999994</v>
       </c>
@@ -5143,7 +7484,7 @@
       <c r="B15" s="42">
         <v>0</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="60">
         <f>196294.329*0.000001</f>
         <v>0.19629432899999999</v>
       </c>
@@ -5168,7 +7509,7 @@
       <c r="C16" s="42">
         <v>0</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="60">
         <f>960161.835*0.000001</f>
         <v>0.96016183499999996</v>
       </c>
@@ -5183,58 +7524,58 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="61">
+        <v>3.32E-2</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="61">
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="61">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="66">
-        <v>3.32E-2</v>
-      </c>
-      <c r="C17" s="66" t="s">
+      <c r="B20" s="61">
+        <v>4.2</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="61" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="61">
+        <v>1.079</v>
+      </c>
+      <c r="C21" s="61" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="66">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="B19" s="66">
-        <v>0.05</v>
-      </c>
-      <c r="C19" s="66" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
-        <v>175</v>
-      </c>
-      <c r="B20" s="66">
-        <v>4.2</v>
-      </c>
-      <c r="C20" s="66" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" s="66">
-        <v>1.079</v>
-      </c>
-      <c r="C21" s="66" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5247,7 +7588,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5276,11 +7617,11 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="56" t="s">
-        <v>166</v>
+      <c r="M1" s="53" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -5310,10 +7651,10 @@
       </c>
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
-      <c r="L2" s="57">
-        <v>0</v>
-      </c>
-      <c r="M2" s="55">
+      <c r="L2" s="54">
+        <v>0</v>
+      </c>
+      <c r="M2" s="52">
         <v>4.7840910259559694E-2</v>
       </c>
     </row>
@@ -5340,14 +7681,14 @@
         <v>65</v>
       </c>
       <c r="H3" s="42">
-        <v>9500</v>
+        <v>5100</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
-      <c r="L3" s="57">
+      <c r="L3" s="54">
         <v>1</v>
       </c>
-      <c r="M3" s="55">
+      <c r="M3" s="52">
         <v>5.4017473473968694E-2</v>
       </c>
     </row>
@@ -5368,7 +7709,7 @@
         <v>66</v>
       </c>
       <c r="F4" s="42">
-        <v>1.0540000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="41" t="s">
         <v>67</v>
@@ -5378,10 +7719,10 @@
       </c>
       <c r="I4" s="39"/>
       <c r="J4" s="39"/>
-      <c r="L4" s="57">
+      <c r="L4" s="54">
         <v>2</v>
       </c>
-      <c r="M4" s="55">
+      <c r="M4" s="52">
         <v>6.2749240514946403E-2</v>
       </c>
     </row>
@@ -5404,10 +7745,10 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
-      <c r="L5" s="57">
+      <c r="L5" s="54">
         <v>3</v>
       </c>
-      <c r="M5" s="55">
+      <c r="M5" s="52">
         <v>7.45220496113803E-2</v>
       </c>
     </row>
@@ -5434,10 +7775,10 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39"/>
-      <c r="L6" s="57">
+      <c r="L6" s="54">
         <v>4</v>
       </c>
-      <c r="M6" s="55">
+      <c r="M6" s="52">
         <v>8.7927589464372208E-2</v>
       </c>
     </row>
@@ -5464,10 +7805,10 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
-      <c r="L7" s="57">
+      <c r="L7" s="54">
         <v>5</v>
       </c>
-      <c r="M7" s="55">
+      <c r="M7" s="52">
         <v>0.10044875221048501</v>
       </c>
     </row>
@@ -5490,10 +7831,10 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
-      <c r="L8" s="57">
+      <c r="L8" s="54">
         <v>6</v>
       </c>
-      <c r="M8" s="55">
+      <c r="M8" s="52">
         <v>0.1121956374547078</v>
       </c>
     </row>
@@ -5501,7 +7842,7 @@
       <c r="A9" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="67">
+      <c r="B9" s="62">
         <v>0.29852699999999999</v>
       </c>
       <c r="C9" s="41" t="s">
@@ -5511,10 +7852,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E9" s="39"/>
-      <c r="L9" s="57">
+      <c r="L9" s="54">
         <v>7</v>
       </c>
-      <c r="M9" s="55">
+      <c r="M9" s="52">
         <v>0.123399555026123</v>
       </c>
     </row>
@@ -5522,16 +7863,16 @@
       <c r="A10" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="68">
+      <c r="B10" s="63">
         <v>4.4114000000000004</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
-      <c r="L10" s="57">
+      <c r="L10" s="54">
         <v>8</v>
       </c>
-      <c r="M10" s="55">
+      <c r="M10" s="52">
         <v>0.134390467436968</v>
       </c>
     </row>
@@ -5539,79 +7880,51 @@
       <c r="A11" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="46">
-        <v>5.0000000000000002E-5</v>
-      </c>
+      <c r="B11" s="63">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="39"/>
-      <c r="L11" s="57">
+      <c r="L11" s="54">
         <v>9</v>
       </c>
-      <c r="M11" s="55">
+      <c r="M11" s="52">
         <v>0.14454002413960801</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="46">
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="46">
-        <v>9.0000000000000006E-5</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B12" s="63">
+        <v>2.21</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="39"/>
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
-      <c r="L12" s="57">
+      <c r="L12" s="54">
         <v>10</v>
       </c>
-      <c r="M12" s="55">
+      <c r="M12" s="52">
         <v>0.154212360607799</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="46">
-        <v>4.4299999999999999E-2</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="46">
-        <v>2.0999999999999999E-3</v>
-      </c>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="46">
-        <v>0.25</v>
-      </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
       <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="42">
-        <v>2.21</v>
-      </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
       <c r="E15" s="39"/>
@@ -5622,11 +7935,11 @@
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
-      <c r="L16" s="56" t="s">
+      <c r="L16" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="56" t="s">
-        <v>165</v>
+      <c r="M16" s="53" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -5637,92 +7950,92 @@
       <c r="E17" s="39"/>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
-      <c r="L17" s="56">
-        <v>0</v>
-      </c>
-      <c r="M17" s="58">
+      <c r="L17" s="53">
+        <v>0</v>
+      </c>
+      <c r="M17" s="55">
         <v>2.0845022250721998E-3</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G18" s="39"/>
-      <c r="L18" s="56">
+      <c r="L18" s="53">
         <v>1</v>
       </c>
-      <c r="M18" s="58">
+      <c r="M18" s="55">
         <v>2.1890376504101377E-3</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G19" s="39"/>
-      <c r="L19" s="56">
+      <c r="L19" s="53">
         <v>2</v>
       </c>
-      <c r="M19" s="58">
+      <c r="M19" s="55">
         <v>2.319156139891804E-3</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L20" s="56">
+      <c r="L20" s="53">
         <v>3</v>
       </c>
-      <c r="M20" s="58">
+      <c r="M20" s="55">
         <v>2.4748576935171998E-3</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L21" s="56">
+      <c r="L21" s="53">
         <v>4</v>
       </c>
-      <c r="M21" s="58">
+      <c r="M21" s="55">
         <v>2.6561423112863251E-3</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L22" s="56">
+      <c r="L22" s="53">
         <v>5</v>
       </c>
-      <c r="M22" s="58">
+      <c r="M22" s="55">
         <v>2.8630099931991793E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L23" s="56">
+      <c r="L23" s="53">
         <v>6</v>
       </c>
-      <c r="M23" s="58">
+      <c r="M23" s="55">
         <v>3.0954607392557638E-3</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L24" s="56">
+      <c r="L24" s="53">
         <v>7</v>
       </c>
-      <c r="M24" s="58">
+      <c r="M24" s="55">
         <v>3.353494549456076E-3</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L25" s="56">
+      <c r="L25" s="53">
         <v>8</v>
       </c>
-      <c r="M25" s="58">
+      <c r="M25" s="55">
         <v>3.6371114238001184E-3</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L26" s="56">
+      <c r="L26" s="53">
         <v>9</v>
       </c>
-      <c r="M26" s="58">
+      <c r="M26" s="55">
         <v>3.9463113622878899E-3</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L27" s="56">
+      <c r="L27" s="53">
         <v>10</v>
       </c>
-      <c r="M27" s="58">
+      <c r="M27" s="55">
         <v>4.2810943649193899E-3</v>
       </c>
     </row>
@@ -5735,11 +8048,435 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37897DA-A06B-43D6-81F3-DFD5F30B10F7}">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="3.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="77"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="77"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="77"/>
+      <c r="M1" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="O1" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="64" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q1" s="64" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="72">
+        <f>SLOPE(N2:N3,M2:M3)</f>
+        <v>-3.4000000000000002E-4</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="72">
+        <f>SLOPE(O2:O3,M2:M3)</f>
+        <v>-4.2000000000000025E-5</v>
+      </c>
+      <c r="F2" s="69"/>
+      <c r="G2" s="71" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" s="72">
+        <f>SLOPE(P2:P3,M2:M3)</f>
+        <v>-3.0000000000000035E-5</v>
+      </c>
+      <c r="I2" s="69"/>
+      <c r="J2" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" s="72">
+        <f>SLOPE(Q2:Q3,M2:M3)</f>
+        <v>-1.3799999999999994E-4</v>
+      </c>
+      <c r="M2" s="53">
+        <v>10</v>
+      </c>
+      <c r="N2" s="65">
+        <v>2.1829999999999999E-2</v>
+      </c>
+      <c r="O2" s="65">
+        <v>2.66E-3</v>
+      </c>
+      <c r="P2" s="65">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="Q2" s="65">
+        <v>8.1899999999999994E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="72">
+        <f>INTERCEPT(N2:N3,M2:M3)</f>
+        <v>2.5229999999999999E-2</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="71" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="72">
+        <f>INTERCEPT(O2:O3,M2:M3)</f>
+        <v>3.0800000000000003E-3</v>
+      </c>
+      <c r="F3" s="69"/>
+      <c r="G3" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="72">
+        <f>INTERCEPT(P2:P3,M2:M3)</f>
+        <v>2.0700000000000002E-3</v>
+      </c>
+      <c r="I3" s="69"/>
+      <c r="J3" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="72">
+        <f>INTERCEPT(Q2:Q3,M2:M3)</f>
+        <v>9.5699999999999986E-3</v>
+      </c>
+      <c r="M3" s="53">
+        <v>15</v>
+      </c>
+      <c r="N3" s="65">
+        <v>2.0129999999999999E-2</v>
+      </c>
+      <c r="O3" s="65">
+        <v>2.4499999999999999E-3</v>
+      </c>
+      <c r="P3" s="65">
+        <v>1.6199999999999999E-3</v>
+      </c>
+      <c r="Q3" s="65">
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="77"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="76" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="77"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="Q4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="72">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="71" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="72">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="Q5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="71" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="72">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="72">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="72">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="C7" s="69"/>
+      <c r="D7" s="71" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="72">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="M8" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="N8" s="64" t="s">
+        <v>200</v>
+      </c>
+      <c r="P8" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q8" s="64" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="69"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="69"/>
+      <c r="M9" s="66">
+        <v>0</v>
+      </c>
+      <c r="N9" s="67">
+        <v>2.6010910259559698E-2</v>
+      </c>
+      <c r="P9" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="68">
+        <v>1.2986457399112525E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M10" s="66">
+        <v>1</v>
+      </c>
+      <c r="N10" s="67">
+        <v>3.2187473473968699E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="68">
+        <v>9.9829656566044261E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M11" s="66">
+        <v>2</v>
+      </c>
+      <c r="N11" s="67">
+        <v>4.0919240514946401E-2</v>
+      </c>
+      <c r="P11" s="66">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="68">
+        <v>7.0882939599435668E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M12" s="66">
+        <v>3</v>
+      </c>
+      <c r="N12" s="67">
+        <v>5.2692049611380298E-2</v>
+      </c>
+      <c r="P12" s="66">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="68">
+        <v>4.2876983381822764E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M13" s="66">
+        <v>4</v>
+      </c>
+      <c r="N13" s="67">
+        <v>6.6097589464372206E-2</v>
+      </c>
+      <c r="P13" s="66">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="68">
+        <v>2.5369892387654705E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M14" s="66">
+        <v>5</v>
+      </c>
+      <c r="N14" s="67">
+        <v>7.8618752210485005E-2</v>
+      </c>
+      <c r="P14" s="66">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="68">
+        <v>8.6442681458535092E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="31"/>
+      <c r="M15" s="66">
+        <v>6</v>
+      </c>
+      <c r="N15" s="67">
+        <v>9.0365637454707798E-2</v>
+      </c>
+      <c r="P15" s="66">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="68">
+        <v>3.8313311342148428E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="31"/>
+      <c r="M16" s="66">
+        <v>7</v>
+      </c>
+      <c r="N16" s="67">
+        <v>0.101569555026123</v>
+      </c>
+      <c r="P16" s="66">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="68">
+        <v>1.5418721241993274E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="31"/>
+      <c r="M17" s="66">
+        <v>8</v>
+      </c>
+      <c r="N17" s="67">
+        <v>0.112560467436968</v>
+      </c>
+      <c r="P17" s="66">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="68">
+        <v>9.5397317936440814E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="31"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A113401-D5F9-4F05-A1A5-75FFBCA62A3E}">
   <dimension ref="A1:AS89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5749,172 +8486,172 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="49">
+      <c r="A2" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="74">
         <v>0</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="49">
-        <v>-5.0196999999999999E-2</v>
+      <c r="A3" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="74">
+        <v>0</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="42">
-        <v>2.4497999999999999E-2</v>
+      <c r="A4" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="74">
+        <v>0</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="42">
-        <v>5.5011999999999998E-2</v>
+      <c r="A5" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="74">
+        <v>0</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="42">
-        <v>-0.63979699999999995</v>
+      <c r="A6" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="74">
+        <v>0</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="42">
-        <v>-6.5456E-2</v>
+      <c r="A7" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="74">
+        <v>0</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="61">
+      <c r="A8" s="73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="75">
         <v>6.9432039999999997</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="42">
+      <c r="A9" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="75">
         <v>-6.8021479999999999</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="42">
-        <v>8.1174999999999997E-2</v>
+      <c r="A10" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="74">
+        <v>0</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="42">
+      <c r="A11" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="74">
         <v>0</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="42">
-        <v>-2.9926999999999999E-2</v>
+      <c r="A12" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="74">
+        <v>0</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="50">
+      <c r="A13" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="74">
         <v>0</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="50">
+      <c r="A14" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="74">
         <v>0</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="50">
+      <c r="A15" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="74">
         <v>0</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="50">
+      <c r="A16" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="75">
         <v>0.377521891</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="60">
+      <c r="A17" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="75">
         <f>1.033214792*-1</f>
         <v>-1.0332147920000001</v>
       </c>
@@ -5922,30 +8659,30 @@
       <c r="D17" s="39"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="50">
+      <c r="A18" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="74">
         <v>0</v>
       </c>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="50">
+      <c r="A19" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="74">
         <v>0</v>
       </c>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="50">
+      <c r="A20" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="74">
         <v>0</v>
       </c>
       <c r="C20" s="39"/>
@@ -6070,12 +8807,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DD314E-C382-46AC-806D-7E5988604C2A}">
   <dimension ref="A1:AD297"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6108,14 +8845,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="71"/>
+      <c r="A1" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="80"/>
       <c r="G1" s="11"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -6143,87 +8880,87 @@
     </row>
     <row r="2" spans="1:30" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="W2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="X2" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="Y2" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="Z2" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B3" s="8">
         <v>-5.3600000000000002E-3</v>
@@ -6303,7 +9040,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B4" s="8">
         <v>-2.988E-2</v>
@@ -6383,7 +9120,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B5" s="8">
         <v>-5.6349999999999997E-2</v>
@@ -6463,7 +9200,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B6" s="8">
         <v>-1.1780000000000001E-2</v>
@@ -6543,7 +9280,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B7" s="8">
         <v>1.828E-3</v>
@@ -6623,7 +9360,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B8" s="8">
         <v>-4.3869999999999998E-4</v>
@@ -6703,7 +9440,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B9" s="8">
         <v>-4.854E-2</v>
@@ -6783,7 +9520,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B10" s="8">
         <v>-5.0139999999999997E-2</v>
@@ -6863,7 +9600,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B11" s="8">
         <v>-0.1295</v>
@@ -6943,7 +9680,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B12" s="8">
         <v>-0.28889999999999999</v>
@@ -7023,7 +9760,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B13" s="8">
         <v>-0.16350000000000001</v>
@@ -7103,7 +9840,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B14" s="8">
         <v>-8.0399999999999999E-2</v>
@@ -7183,7 +9920,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B15" s="16">
         <v>0</v>
@@ -7263,7 +10000,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B16" s="16">
         <v>0</v>
@@ -7343,7 +10080,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B17" s="16">
         <v>0</v>
@@ -7423,7 +10160,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -7503,7 +10240,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B19" s="16">
         <v>0</v>
@@ -7583,7 +10320,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B20" s="16">
         <v>0</v>
@@ -7663,7 +10400,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B21" s="16">
         <v>0</v>
@@ -7743,7 +10480,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19">
@@ -7810,7 +10547,7 @@
         <v>14000</v>
       </c>
       <c r="X22" s="16" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="Y22" s="20">
         <v>4.4000000000000004</v>
@@ -7821,7 +10558,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B23" s="24">
         <v>0</v>
@@ -7901,7 +10638,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B24" s="24">
         <v>0</v>
@@ -7981,7 +10718,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B25" s="19">
         <v>1.7618</v>
@@ -8061,7 +10798,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B26" s="27">
         <v>1.268</v>
@@ -8141,7 +10878,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B27" s="8">
         <v>0.68540000000000001</v>
@@ -8221,7 +10958,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B28" s="8">
         <v>0.81169999999999998</v>
@@ -8301,7 +11038,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B29" s="8">
         <v>0.77680000000000005</v>
@@ -8381,7 +11118,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B30" s="8">
         <v>0.96760000000000002</v>
@@ -8461,7 +11198,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B31">
         <v>-3.3240000000000001E-3</v>
@@ -8541,7 +11278,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B32" s="8">
         <v>0.88239999999999996</v>
@@ -8621,7 +11358,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B33" s="8">
         <v>-4.854E-2</v>
@@ -8701,7 +11438,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B34">
         <v>1.2080000000000001E-3</v>
@@ -8781,7 +11518,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B35" s="35">
         <v>0</v>
@@ -8861,9 +11598,9 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B36" s="51">
+        <v>156</v>
+      </c>
+      <c r="B36" s="48">
         <f>Y36</f>
         <v>4.7</v>
       </c>
@@ -8941,8 +11678,8 @@
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A37" s="52" t="s">
-        <v>163</v>
+      <c r="A37" s="49" t="s">
+        <v>157</v>
       </c>
       <c r="B37" s="8">
         <v>-5.0700000000000002E-2</v>
@@ -9022,34 +11759,34 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B38" s="51">
+        <v>158</v>
+      </c>
+      <c r="B38" s="48">
         <f>Y38</f>
         <v>5.1100000000000003</v>
       </c>
-      <c r="C38" s="54">
+      <c r="C38" s="51">
         <v>0</v>
       </c>
       <c r="D38" s="17">
         <v>-2.9221700999999999E-2</v>
       </c>
-      <c r="E38" s="54">
-        <v>0</v>
-      </c>
-      <c r="F38" s="54">
+      <c r="E38" s="51">
+        <v>0</v>
+      </c>
+      <c r="F38" s="51">
         <v>0</v>
       </c>
       <c r="G38" s="17">
         <v>-2.54155E-4</v>
       </c>
-      <c r="H38" s="54">
-        <v>0</v>
-      </c>
-      <c r="I38" s="54">
-        <v>0</v>
-      </c>
-      <c r="J38" s="54">
+      <c r="H38" s="51">
+        <v>0</v>
+      </c>
+      <c r="I38" s="51">
+        <v>0</v>
+      </c>
+      <c r="J38" s="51">
         <v>0</v>
       </c>
       <c r="K38" s="29">
@@ -9102,34 +11839,34 @@
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A39" s="63" t="s">
-        <v>167</v>
+      <c r="A39" s="58" t="s">
+        <v>161</v>
       </c>
       <c r="B39" s="16">
         <v>2.137</v>
       </c>
-      <c r="C39" s="54">
+      <c r="C39" s="51">
         <v>-1.577</v>
       </c>
       <c r="D39" s="17">
         <v>3.49</v>
       </c>
-      <c r="E39" s="54">
+      <c r="E39" s="51">
         <v>-0.2586</v>
       </c>
-      <c r="F39" s="54">
+      <c r="F39" s="51">
         <v>-0.71099999999999997</v>
       </c>
       <c r="G39" s="17">
         <v>1.9770000000000001</v>
       </c>
-      <c r="H39" s="54">
+      <c r="H39" s="51">
         <v>-1.383E-2</v>
       </c>
-      <c r="I39" s="54">
+      <c r="I39" s="51">
         <v>1.324E-2</v>
       </c>
-      <c r="J39" s="54">
+      <c r="J39" s="51">
         <v>-0.30499999999999999</v>
       </c>
       <c r="K39" s="29">
@@ -9988,21 +12725,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010026F0D136D79F25469E9BD90619CDB412" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4a869207c6945743f5de18208a2cfcba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f9188d7-3b18-4187-a3cb-7b6899b4ef8f" xmlns:ns3="85078965-a7f2-4dbb-adf6-2b7faeeb76ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89813893f4c0c91941f9d9d5434200cd" ns2:_="" ns3:_="">
     <xsd:import namespace="4f9188d7-3b18-4187-a3cb-7b6899b4ef8f"/>
@@ -10225,24 +12947,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D6E2B2-1F78-45C8-93F5-31B8FF78EAA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BAFCAE4-A011-4769-B47E-67DBBC3AE6CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51AA6EA-A3F6-4587-80EF-6E5C51392FC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10259,4 +12979,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D6E2B2-1F78-45C8-93F5-31B8FF78EAA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BAFCAE4-A011-4769-B47E-67DBBC3AE6CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>